<commit_message>
Update export report v2
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon.xlsx
@@ -472,19 +472,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="34" style="3" customWidth="1"/>
     <col min="3" max="3" width="21" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="26" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="20.6640625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>